<commit_message>
Project Commit v1.0.0 by Naveen
</commit_message>
<xml_diff>
--- a/Thedal/resource/TestCase/Google_Automation_Testcase.xlsx
+++ b/Thedal/resource/TestCase/Google_Automation_Testcase.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22943" windowHeight="9887"/>
+    <workbookView windowWidth="28695" windowHeight="13035"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <oleSize ref="A1:H6"/>
 </workbook>
 </file>
 
@@ -53,13 +54,13 @@
     <t>Click Gmail</t>
   </si>
   <si>
-    <t>EnterInput</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>//a[@href='https://mail.google.com/mail/?tab=wm']</t>
+    <t>Click</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>//div[@class='gb_Q gb_R'][1]/a[@class='gb_P']</t>
   </si>
 </sst>
 </file>
@@ -67,10 +68,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -98,7 +99,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -106,15 +114,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -128,6 +128,60 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -136,90 +190,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -234,13 +235,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -252,169 +409,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -428,17 +429,61 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -458,31 +503,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -495,183 +526,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -741,6 +742,11 @@
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1000,23 +1006,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="37" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.8611111111111" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1388888888889" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.712962962963" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.4259259259259" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.1388888888889" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.13888888888889" style="1"/>
+    <col min="2" max="2" width="16.8571428571429" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1428571428571" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7142857142857" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.4285714285714" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.1428571428571" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1087,7 +1093,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -1095,7 +1101,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>